<commit_message>
Abnahmetest Durchlauf 2, Frontend. Betrifft #162
</commit_message>
<xml_diff>
--- a/documents/project management/Test/Durchlauf 2/Abnahmetest_Go Happy_Frontend.xlsx
+++ b/documents/project management/Test/Durchlauf 2/Abnahmetest_Go Happy_Frontend.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28760" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Frontend" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Es öffnet sich ein Pop-Up, in dem das Löschen bestätigt werden muss. Mit Bestätigung ist die Route entfernt.</t>
   </si>
   <si>
-    <t>Es öffnet sich ein Pop-Up, in dem das Löschen bestätigt werden muss. Wird der Vorgang jeder abgebrochen gelangt der Anwender wieder zurück zu der "Offline Routen Ansicht".</t>
-  </si>
-  <si>
     <t>Die Bar wird aus der aktuellen Route entfernt und kann durch eine neue Bar aus einer Liste ausgetauscht werden.</t>
   </si>
   <si>
@@ -210,7 +207,37 @@
     <t>Der Anwender hat sich eine Route erstellen lassen und möchte eine Bar entfernen und swipt auf der gewünschte Bar nach links.</t>
   </si>
   <si>
-    <t>Es erscheint ein Pop Up fenster in welches man einen Text zur Fehlermeldung ientragen kann. Dieser kann anschließend abgeschickt oder aber auch verworfen werden. Es folgt eine Bestätigung.</t>
+    <t xml:space="preserve">Sobald die Einstellungen vorgenommen wurden und es auf den Zurückpfeil geklickt wurde, tauchen bereits andere Bars in der "Auswahlübersicht" auf. Beim Aktualisieren wird dann letztendlich eine neue Route generiert. </t>
+  </si>
+  <si>
+    <t>Wird wohl bereits aktualisiert, nach dem man auf den Zurückpfeil geklickt hat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.o. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bereits nach dem Klick auf den Zurückpfeil, tauchen Bars in der "Auswahlübersicht" auf. Nach dem Klick auf den Aktualisierungsbutton, wird letztendlich eine neue Route erstellt. </t>
+  </si>
+  <si>
+    <t>Hat noch einen Schönheitsfehler. Die Fenster mit dem weißen Hintergrund sind wohl nicht dynamisch und deswegen u.U. zu klein für die Informationen</t>
+  </si>
+  <si>
+    <t>Scheint wohl zu funktionieren. Bisher aber nur eine Route drin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Link wird angezeigt. Es erfolgt jedoch kein Kopieren des Linkes in die Zwischenablage nach Betätigen des Kopierbuttons. </t>
+  </si>
+  <si>
+    <t>Nach Routen fehlt ein Komma</t>
+  </si>
+  <si>
+    <t>Es erscheint ein Pop Up fenster in welches man einen Text zur Fehlermeldung eintragen kann. Dieser kann anschließend abgeschickt oder aber auch verworfen werden. Es folgt eine Bestätigung.</t>
+  </si>
+  <si>
+    <t>Es öffnet sich ein Pop-Up, in dem das Löschen bestätigt werden muss. Wird der Vorgang jedoch abgebrochen gelangt der Anwender wieder zurück zu der "Offline Routen Ansicht".</t>
+  </si>
+  <si>
+    <t>Man kann eine Bar ohne Begründung melden. Evtl. nicht ganz sinnvoll</t>
   </si>
 </sst>
 </file>
@@ -345,8 +372,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="153">
+  <cellStyleXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -531,7 +564,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="153">
+  <cellStyles count="159">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -608,6 +641,9 @@
     <cellStyle name="Besuchter Link" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -684,6 +720,9 @@
     <cellStyle name="Link" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -1257,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1302,7 +1341,9 @@
       <c r="C3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" ht="45">
@@ -1310,78 +1351,100 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:5" ht="45">
+    <row r="5" spans="1:5" ht="150">
       <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:5" ht="45">
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60">
       <c r="A6" s="6">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="45">
       <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:5" ht="45">
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="120">
       <c r="A8" s="6">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" ht="45">
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60">
       <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="7"/>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6">
@@ -1393,10 +1456,12 @@
       <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="8">
+        <v>1</v>
+      </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="105">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1406,8 +1471,12 @@
       <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="7"/>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6">
@@ -1419,10 +1488,12 @@
       <c r="C12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="60">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1432,8 +1503,12 @@
       <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="7"/>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="30">
       <c r="A14" s="6">
@@ -1445,7 +1520,9 @@
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
       <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" ht="30">
@@ -1458,7 +1535,9 @@
       <c r="C15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" ht="30">
@@ -1471,10 +1550,12 @@
       <c r="C16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="8"/>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="1:5" ht="30">
+    <row r="17" spans="1:5" ht="90">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -1484,8 +1565,12 @@
       <c r="C17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="7"/>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="30">
       <c r="A18" s="6">
@@ -1497,7 +1582,9 @@
       <c r="C18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
       <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="30">
@@ -1510,7 +1597,9 @@
       <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
       <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" ht="45">
@@ -1523,7 +1612,9 @@
       <c r="C20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="8"/>
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
       <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="30">
@@ -1536,7 +1627,9 @@
       <c r="C21" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="8"/>
+      <c r="D21" s="8">
+        <v>1</v>
+      </c>
       <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" ht="30">
@@ -1549,7 +1642,9 @@
       <c r="C22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="8"/>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="30">
@@ -1560,9 +1655,11 @@
         <v>30</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="8"/>
+        <v>71</v>
+      </c>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
       <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" ht="45">
@@ -1575,20 +1672,26 @@
       <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="30">
       <c r="A25" s="4">
         <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1</v>
+      </c>
       <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" ht="30">
@@ -1601,7 +1704,9 @@
       <c r="C26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="8"/>
+      <c r="D26" s="8">
+        <v>1</v>
+      </c>
       <c r="E26" s="9"/>
     </row>
     <row r="27" spans="1:5" ht="45">
@@ -1609,13 +1714,17 @@
         <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="D27" s="8">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="30">
       <c r="A28" s="6">
@@ -1625,9 +1734,11 @@
         <v>34</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="8"/>
+        <v>48</v>
+      </c>
+      <c r="D28" s="8">
+        <v>1</v>
+      </c>
       <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5" ht="45">
@@ -1638,9 +1749,11 @@
         <v>35</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="8"/>
+        <v>49</v>
+      </c>
+      <c r="D29" s="8">
+        <v>1</v>
+      </c>
       <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" ht="30">
@@ -1651,9 +1764,11 @@
         <v>32</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="8"/>
+        <v>50</v>
+      </c>
+      <c r="D30" s="8">
+        <v>1</v>
+      </c>
       <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5" ht="30">
@@ -1664,9 +1779,11 @@
         <v>33</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="8"/>
+        <v>51</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
       <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" ht="30">
@@ -1677,9 +1794,11 @@
         <v>36</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="8"/>
+        <v>52</v>
+      </c>
+      <c r="D32" s="8">
+        <v>1</v>
+      </c>
       <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5">
@@ -1690,13 +1809,15 @@
         <v>37</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="8"/>
+        <v>53</v>
+      </c>
+      <c r="D33" s="8">
+        <v>1</v>
+      </c>
       <c r="E33" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:E33">
+  <conditionalFormatting sqref="D3:E8 D9 D10:E33">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>